<commit_message>
Reworked operation form. Data now passed to TabbedResultsControl
</commit_message>
<xml_diff>
--- a/GhdAutoStoreUtilities/GhdAutoStoreUtilities.Tests/TestFiles/synq_tus_simple.xlsx
+++ b/GhdAutoStoreUtilities/GhdAutoStoreUtilities.Tests/TestFiles/synq_tus_simple.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h4dottd\Documents\NET Projects\AutoStoreMissingBinFinder\AutoStoreMissingBinFinder.Tests\TestFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\GHD-AutoStore-Utilities\GhdAutoStoreUtilities\GhdAutoStoreUtilities.Tests\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF02947-7EC4-49F8-97F2-E00EB370CE37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32E30C4-544C-4BF9-AB66-2F35746F1743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6015" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
   <si>
     <t>TU</t>
+  </si>
+  <si>
+    <t>GRID1</t>
+  </si>
+  <si>
+    <t>PORT7</t>
+  </si>
+  <si>
+    <t>Current_Location</t>
   </si>
 </sst>
 </file>
@@ -354,42 +363,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10001</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10002</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10003</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10004</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10005</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added logic to determine mismatched locations
</commit_message>
<xml_diff>
--- a/GhdAutoStoreUtilities/GhdAutoStoreUtilities.Tests/TestFiles/synq_tus_simple.xlsx
+++ b/GhdAutoStoreUtilities/GhdAutoStoreUtilities.Tests/TestFiles/synq_tus_simple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\GHD-AutoStore-Utilities\GhdAutoStoreUtilities\GhdAutoStoreUtilities.Tests\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32E30C4-544C-4BF9-AB66-2F35746F1743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90288A9C-A2AA-489D-9B09-6FF110D23867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6015" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
     <t>PORT7</t>
   </si>
   <si>
-    <t>Current_Location</t>
+    <t>CURRENT_LOCATION</t>
   </si>
 </sst>
 </file>

</xml_diff>